<commit_message>
16th Commit: tesla_graph.py file developed. It yielded the tesla histogram and fitted normal curve shown in tsla_hist_fitted_normal.png file. Testla stock price history raw data also added to the Repository in this commit.
</commit_message>
<xml_diff>
--- a/data/processed/fat_tails.xlsx
+++ b/data/processed/fat_tails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Python\Python Projects\fat_tails\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26343B62-72C4-418F-AEEF-B0AF72624D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37799DAB-710E-4849-BDC0-928854672D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="461">
   <si>
     <t>Date</t>
   </si>
@@ -1416,6 +1416,9 @@
   </si>
   <si>
     <t>annualized return</t>
+  </si>
+  <si>
+    <t>z-score</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1431,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1456,6 +1459,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1477,7 +1486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1543,12 +1552,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1578,6 +1598,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18886,10 +18909,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I236"/>
+  <dimension ref="A1:J236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="G231" sqref="G231"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18898,10 +18922,10 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="7" max="7" width="8.90625" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -18929,8 +18953,11 @@
       <c r="I1" s="5" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="17">
         <v>45660</v>
       </c>
@@ -18958,8 +18985,12 @@
       <c r="I2" s="20">
         <v>7.8955036400145477</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="20">
+        <f>(H2-C$227)/C$228</f>
+        <v>1.9140355412096945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="17">
         <v>45663</v>
       </c>
@@ -18987,8 +19018,12 @@
       <c r="I3" s="20">
         <v>0.1485106604134106</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="20">
+        <f t="shared" ref="J3:J66" si="0">(H3-C$227)/C$228</f>
+        <v>3.1578072843844736E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="17">
         <v>45664</v>
       </c>
@@ -19016,8 +19051,12 @@
       <c r="I4" s="20">
         <v>-4.145066389130184</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.0117268848603618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="17">
         <v>45665</v>
       </c>
@@ -19045,8 +19084,12 @@
       <c r="I5" s="20">
         <v>0.14696569223229569</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="20">
+        <f t="shared" si="0"/>
+        <v>3.1202657905611872E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="17">
         <v>45667</v>
       </c>
@@ -19074,8 +19117,12 @@
       <c r="I6" s="20">
         <v>-5.0653430320193517E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.6817211754834475E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="17">
         <v>45670</v>
       </c>
@@ -19103,8 +19150,12 @@
       <c r="I7" s="20">
         <v>2.1478176683598589</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="20">
+        <f t="shared" si="0"/>
+        <v>0.51739372009885842</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="17">
         <v>45671</v>
       </c>
@@ -19132,8 +19183,12 @@
       <c r="I8" s="20">
         <v>-1.7382607818861551</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.42689233006067551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="17">
         <v>45672</v>
       </c>
@@ -19161,8 +19216,12 @@
       <c r="I9" s="20">
         <v>7.7314193020332418</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="20">
+        <f t="shared" si="0"/>
+        <v>1.8741643565722357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="17">
         <v>45673</v>
       </c>
@@ -19190,8 +19249,12 @@
       <c r="I10" s="20">
         <v>-3.4205985539776229</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.83568698260863772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>45674</v>
       </c>
@@ -19219,8 +19282,12 @@
       <c r="I11" s="20">
         <v>3.0181270260479018</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="20">
+        <f t="shared" si="0"/>
+        <v>0.72887194842337832</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
         <v>45678</v>
       </c>
@@ -19248,8 +19315,12 @@
       <c r="I12" s="20">
         <v>-0.57138309867241321</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.14335036542754859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="17">
         <v>45679</v>
       </c>
@@ -19277,8 +19348,12 @@
       <c r="I13" s="20">
         <v>-2.1354990595606971</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.52341806133450575</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="17">
         <v>45680</v>
       </c>
@@ -19306,8 +19381,12 @@
       <c r="I14" s="20">
         <v>-0.65982909878338736</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.16484203760208077</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
         <v>45681</v>
       </c>
@@ -19335,8 +19414,12 @@
       <c r="I15" s="20">
         <v>-1.4164542768650801</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.34869591755058904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
         <v>45684</v>
       </c>
@@ -19364,8 +19447,12 @@
       <c r="I16" s="20">
         <v>-2.3466668513776971</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.57473014949967449</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
         <v>45685</v>
       </c>
@@ -19393,8 +19480,12 @@
       <c r="I17" s="20">
         <v>0.236406729488047</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="20">
+        <f t="shared" si="0"/>
+        <v>5.293611616532827E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="17">
         <v>45686</v>
       </c>
@@ -19422,8 +19513,12 @@
       <c r="I18" s="20">
         <v>-2.284173038351355</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.55954465167259992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
         <v>45687</v>
       </c>
@@ -19451,8 +19546,12 @@
       <c r="I19" s="20">
         <v>2.832792223174724</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="20">
+        <f t="shared" si="0"/>
+        <v>0.68383707040872332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="17">
         <v>45688</v>
       </c>
@@ -19480,8 +19579,12 @@
       <c r="I20" s="20">
         <v>1.073462251138994</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20" s="20">
+        <f t="shared" si="0"/>
+        <v>0.25633392771850527</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="17">
         <v>45691</v>
       </c>
@@ -19509,8 +19612,12 @@
       <c r="I21" s="20">
         <v>-5.3090052894495674</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.2945547487034197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
         <v>45692</v>
       </c>
@@ -19538,8 +19645,12 @@
       <c r="I22" s="20">
         <v>2.1988538793356982</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22" s="20">
+        <f t="shared" si="0"/>
+        <v>0.52979511206623697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="17">
         <v>45693</v>
       </c>
@@ -19567,8 +19678,12 @@
       <c r="I23" s="20">
         <v>-3.645358066385942</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.89030175040736759</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
         <v>45694</v>
       </c>
@@ -19596,8 +19711,12 @@
       <c r="I24" s="20">
         <v>-1.0232783410686179</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.2531573029331935</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="17">
         <v>45695</v>
       </c>
@@ -19625,8 +19744,12 @@
       <c r="I25" s="20">
         <v>-3.4517109834953108</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.84324705468548022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="17">
         <v>45698</v>
       </c>
@@ -19654,8 +19777,12 @@
       <c r="I26" s="20">
         <v>-3.0577240036170501</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.74751136282882857</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="17">
         <v>45699</v>
       </c>
@@ -19683,8 +19810,12 @@
       <c r="I27" s="20">
         <v>-6.5479858762172061</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.5956171434754787</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="17">
         <v>45700</v>
       </c>
@@ -19712,8 +19843,12 @@
       <c r="I28" s="20">
         <v>2.4091028400576402</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J28" s="20">
+        <f t="shared" si="0"/>
+        <v>0.5808839316081329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="17">
         <v>45701</v>
       </c>
@@ -19741,8 +19876,12 @@
       <c r="I29" s="20">
         <v>5.6134310996597856</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="20">
+        <f t="shared" si="0"/>
+        <v>1.3595101262189833</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="17">
         <v>45702</v>
       </c>
@@ -19770,8 +19909,12 @@
       <c r="I30" s="20">
         <v>-2.809856996767603E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J30" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.1336560690564192E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="17">
         <v>45706</v>
       </c>
@@ -19799,8 +19942,12 @@
       <c r="I31" s="20">
         <v>-0.48735922930660758</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.12293323573282142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="17">
         <v>45707</v>
       </c>
@@ -19828,8 +19975,12 @@
       <c r="I32" s="20">
         <v>1.805077905329606</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J32" s="20">
+        <f t="shared" si="0"/>
+        <v>0.43411069295256799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="17">
         <v>45708</v>
       </c>
@@ -19857,8 +20008,12 @@
       <c r="I33" s="20">
         <v>-1.7232159651467049</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J33" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.4232365596597023</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
         <v>45709</v>
       </c>
@@ -19886,8 +20041,12 @@
       <c r="I34" s="20">
         <v>-4.7972214357226104</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J34" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.1701953565916476</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="17">
         <v>45712</v>
       </c>
@@ -19915,8 +20074,12 @@
       <c r="I35" s="20">
         <v>-2.1756577643202322</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J35" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.53317630610038369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="17">
         <v>45713</v>
       </c>
@@ -19944,8 +20107,12 @@
       <c r="I36" s="20">
         <v>-8.7624905167203622</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J36" s="20">
+        <f t="shared" si="0"/>
+        <v>-2.13372409803485</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="17">
         <v>45714</v>
       </c>
@@ -19973,8 +20140,12 @@
       <c r="I37" s="20">
         <v>-4.0436775903929467</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.98709021591098833</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="17">
         <v>45715</v>
       </c>
@@ -20002,8 +20173,12 @@
       <c r="I38" s="20">
         <v>-3.0905995406173279</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.75549985595327929</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="17">
         <v>45716</v>
       </c>
@@ -20031,8 +20206,12 @@
       <c r="I39" s="20">
         <v>3.837459704843277</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39" s="20">
+        <f t="shared" si="0"/>
+        <v>0.92796325060162865</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>45719</v>
       </c>
@@ -20060,8 +20239,12 @@
       <c r="I40" s="20">
         <v>-2.8843991904533111</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.70539481646660451</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="17">
         <v>45720</v>
       </c>
@@ -20089,8 +20272,12 @@
       <c r="I41" s="20">
         <v>-4.5311241089652832</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J41" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.1055358298068034</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="17">
         <v>45721</v>
       </c>
@@ -20118,8 +20305,12 @@
       <c r="I42" s="20">
         <v>2.5621026234838511</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J42" s="20">
+        <f t="shared" si="0"/>
+        <v>0.6180616579501359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="17">
         <v>45722</v>
       </c>
@@ -20147,8 +20338,12 @@
       <c r="I43" s="20">
         <v>-5.7706543886981869</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J43" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.4067317955825402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="17">
         <v>45723</v>
       </c>
@@ -20176,8 +20371,12 @@
       <c r="I44" s="20">
         <v>-0.29651051907172271</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J44" s="20">
+        <f t="shared" si="0"/>
+        <v>-7.6558522233578452E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="17">
         <v>45726</v>
       </c>
@@ -20205,8 +20404,12 @@
       <c r="I45" s="20">
         <v>-16.754566208265999</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J45" s="20">
+        <f t="shared" si="0"/>
+        <v>-4.0757347094953298</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="17">
         <v>45727</v>
       </c>
@@ -20234,8 +20437,12 @@
       <c r="I46" s="20">
         <v>3.7245044422890028</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J46" s="20">
+        <f t="shared" si="0"/>
+        <v>0.90051602325207336</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="17">
         <v>45728</v>
       </c>
@@ -20263,8 +20470,12 @@
       <c r="I47" s="20">
         <v>7.3193709752532392</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J47" s="20">
+        <f t="shared" si="0"/>
+        <v>1.7740399015589043</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="17">
         <v>45729</v>
       </c>
@@ -20292,8 +20503,12 @@
       <c r="I48" s="20">
         <v>-3.032333320518898</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J48" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.74134162946894533</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="17">
         <v>45730</v>
       </c>
@@ -20321,8 +20536,12 @@
       <c r="I49" s="20">
         <v>3.7912664309924611</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J49" s="20">
+        <f t="shared" si="0"/>
+        <v>0.91673865370607088</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="17">
         <v>45733</v>
       </c>
@@ -20350,8 +20569,12 @@
       <c r="I50" s="20">
         <v>-4.9068225066559679</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J50" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.1968275421457921</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="17">
         <v>45734</v>
       </c>
@@ -20379,8 +20602,12 @@
       <c r="I51" s="20">
         <v>-5.4835457878221687</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J51" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.3369666968694964</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="17">
         <v>45735</v>
       </c>
@@ -20408,8 +20635,12 @@
       <c r="I52" s="20">
         <v>4.5761176944529591</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J52" s="20">
+        <f t="shared" si="0"/>
+        <v>1.1074512471404403</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="17">
         <v>45736</v>
       </c>
@@ -20437,8 +20668,12 @@
       <c r="I53" s="20">
         <v>0.16944848585497799</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J53" s="20">
+        <f t="shared" si="0"/>
+        <v>3.6665797329668182E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="17">
         <v>45737</v>
       </c>
@@ -20466,8 +20701,12 @@
       <c r="I54" s="20">
         <v>5.1354665567875148</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J54" s="20">
+        <f t="shared" si="0"/>
+        <v>1.2433685567463979</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="17">
         <v>45740</v>
       </c>
@@ -20495,8 +20734,12 @@
       <c r="I55" s="20">
         <v>11.273544918666349</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J55" s="20">
+        <f t="shared" si="0"/>
+        <v>2.7348726131149297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="17">
         <v>45741</v>
       </c>
@@ -20524,8 +20767,12 @@
       <c r="I56" s="20">
         <v>3.442346485841429</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J56" s="20">
+        <f t="shared" si="0"/>
+        <v>0.83195389162601241</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="17">
         <v>45742</v>
       </c>
@@ -20553,8 +20800,12 @@
       <c r="I57" s="20">
         <v>-5.7423842928042861</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J57" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.399862387892741</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="17">
         <v>45743</v>
       </c>
@@ -20582,8 +20833,12 @@
       <c r="I58" s="20">
         <v>0.39252421131618531</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J58" s="20">
+        <f t="shared" si="0"/>
+        <v>9.0871418337885521E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="17">
         <v>45744</v>
       </c>
@@ -20611,8 +20866,12 @@
       <c r="I59" s="20">
         <v>-3.570476901722984</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J59" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.87210622499113366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="17">
         <v>45747</v>
       </c>
@@ -20640,8 +20899,12 @@
       <c r="I60" s="20">
         <v>-1.6797471719459369</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J60" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.41267398981910725</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="17">
         <v>45748</v>
       </c>
@@ -20669,8 +20932,12 @@
       <c r="I61" s="20">
         <v>3.5256295477733439</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J61" s="20">
+        <f t="shared" si="0"/>
+        <v>0.85219101102639472</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="17">
         <v>45749</v>
       </c>
@@ -20698,8 +20965,12 @@
       <c r="I62" s="20">
         <v>5.1896554243263324</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J62" s="20">
+        <f t="shared" si="0"/>
+        <v>1.2565360190984789</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="17">
         <v>45750</v>
       </c>
@@ -20727,8 +20998,12 @@
       <c r="I63" s="20">
         <v>-5.6301683254252248</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J63" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.3725948033707414</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="17">
         <v>45751</v>
       </c>
@@ -20756,8 +21031,12 @@
       <c r="I64" s="20">
         <v>-11.003569949247369</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J64" s="20">
+        <f t="shared" si="0"/>
+        <v>-2.6782885149731461</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="17">
         <v>45754</v>
       </c>
@@ -20785,8 +21064,12 @@
       <c r="I65" s="20">
         <v>-2.5978783713479969</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J65" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.63577254403298877</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="17">
         <v>45755</v>
       </c>
@@ -20814,8 +21097,12 @@
       <c r="I66" s="20">
         <v>-5.023576253203375</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J66" s="20">
+        <f t="shared" si="0"/>
+        <v>-1.225197770791485</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="17">
         <v>45756</v>
       </c>
@@ -20843,8 +21130,12 @@
       <c r="I67" s="20">
         <v>20.449053790685209</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J67" s="20">
+        <f t="shared" ref="J67:J130" si="1">(H67-C$227)/C$228</f>
+        <v>4.9644480429197353</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="17">
         <v>45757</v>
       </c>
@@ -20872,8 +21163,12 @@
       <c r="I68" s="20">
         <v>-7.5521959550307551</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J68" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.8396321784249685</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="17">
         <v>45758</v>
       </c>
@@ -20901,8 +21196,12 @@
       <c r="I69" s="20">
         <v>-3.5664045076955767E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J69" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.3174910765064047E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="17">
         <v>45761</v>
       </c>
@@ -20930,8 +21229,12 @@
       <c r="I70" s="20">
         <v>1.585225699826941E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J70" s="20">
+        <f t="shared" si="1"/>
+        <v>-6.5686049195127127E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="17">
         <v>45762</v>
       </c>
@@ -20959,8 +21262,12 @@
       <c r="I71" s="20">
         <v>0.6950231350284759</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J71" s="20">
+        <f t="shared" si="1"/>
+        <v>0.16437624267608328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="17">
         <v>45763</v>
       </c>
@@ -20988,8 +21295,12 @@
       <c r="I72" s="20">
         <v>-5.0690753136140536</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J72" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.236253679361331</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="17">
         <v>45764</v>
       </c>
@@ -21017,8 +21328,12 @@
       <c r="I73" s="20">
         <v>-7.4546512190748315E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J73" s="20">
+        <f t="shared" si="1"/>
+        <v>-2.2623039968172842E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="17">
         <v>45768</v>
       </c>
@@ -21046,8 +21361,12 @@
       <c r="I74" s="20">
         <v>-5.9180787487503146</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J74" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.4425547385398827</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="17">
         <v>45769</v>
       </c>
@@ -21075,8 +21394,12 @@
       <c r="I75" s="20">
         <v>4.499437691527957</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J75" s="20">
+        <f t="shared" si="1"/>
+        <v>1.0888186183823443</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="17">
         <v>45770</v>
       </c>
@@ -21104,8 +21427,12 @@
       <c r="I76" s="20">
         <v>5.2271930381594336</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J76" s="20">
+        <f t="shared" si="1"/>
+        <v>1.2656573596871206</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="17">
         <v>45771</v>
       </c>
@@ -21133,8 +21460,12 @@
       <c r="I77" s="20">
         <v>3.4378691821057439</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J77" s="20">
+        <f t="shared" si="1"/>
+        <v>0.83086594254982593</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="17">
         <v>45772</v>
       </c>
@@ -21162,8 +21493,12 @@
       <c r="I78" s="20">
         <v>9.3518488772072139</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J78" s="20">
+        <f t="shared" si="1"/>
+        <v>2.267915811334003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="17">
         <v>45775</v>
       </c>
@@ -21191,8 +21526,12 @@
       <c r="I79" s="20">
         <v>0.32584160707696358</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J79" s="20">
+        <f t="shared" si="1"/>
+        <v>7.466807767516169E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="17">
         <v>45776</v>
       </c>
@@ -21220,8 +21559,12 @@
       <c r="I80" s="20">
         <v>2.128439436516667</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J80" s="20">
+        <f t="shared" si="1"/>
+        <v>0.51268496441094269</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="17">
         <v>45777</v>
       </c>
@@ -21249,8 +21592,12 @@
       <c r="I81" s="20">
         <v>-3.4382250789148192</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J81" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.83997008749807434</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="17">
         <v>45778</v>
       </c>
@@ -21278,8 +21625,12 @@
       <c r="I82" s="20">
         <v>-0.58292622590870424</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J82" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.14615525322484876</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="17">
         <v>45779</v>
       </c>
@@ -21307,8 +21658,12 @@
       <c r="I83" s="20">
         <v>2.3568631840698329</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J83" s="20">
+        <f t="shared" si="1"/>
+        <v>0.56819011210706338</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="17">
         <v>45782</v>
       </c>
@@ -21336,8 +21691,12 @@
       <c r="I84" s="20">
         <v>-2.4495911767336329</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J84" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.59973993916296309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="17">
         <v>45783</v>
       </c>
@@ -21365,8 +21724,12 @@
       <c r="I85" s="20">
         <v>-1.767472803358104</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J85" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.43399061814880591</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="17">
         <v>45784</v>
       </c>
@@ -21394,8 +21757,12 @@
       <c r="I86" s="20">
         <v>0.31546339412920171</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J86" s="20">
+        <f t="shared" si="1"/>
+        <v>7.2146254753255354E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="17">
         <v>45785</v>
       </c>
@@ -21423,8 +21790,12 @@
       <c r="I87" s="20">
         <v>3.0659752141498928</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J87" s="20">
+        <f t="shared" si="1"/>
+        <v>0.74049867627475741</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="17">
         <v>45786</v>
       </c>
@@ -21452,8 +21823,12 @@
       <c r="I88" s="20">
         <v>4.6108187543354546</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J88" s="20">
+        <f t="shared" si="1"/>
+        <v>1.1158833277564959</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="17">
         <v>45789</v>
       </c>
@@ -21481,8 +21856,12 @@
       <c r="I89" s="20">
         <v>6.5280048592353648</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J89" s="20">
+        <f t="shared" si="1"/>
+        <v>1.5817442509455455</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="17">
         <v>45790</v>
       </c>
@@ -21510,8 +21889,12 @@
       <c r="I90" s="20">
         <v>4.8104913929038</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J90" s="20">
+        <f t="shared" si="1"/>
+        <v>1.1644021854204989</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="17">
         <v>45791</v>
       </c>
@@ -21539,8 +21922,12 @@
       <c r="I91" s="20">
         <v>3.9931964652091589</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J91" s="20">
+        <f t="shared" si="1"/>
+        <v>0.96580604049724428</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="17">
         <v>45792</v>
       </c>
@@ -21568,8 +21955,12 @@
       <c r="I92" s="20">
         <v>-1.407698842920861</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J92" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.34656841697578827</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="17">
         <v>45793</v>
       </c>
@@ -21597,8 +21988,12 @@
       <c r="I93" s="20">
         <v>2.067048191469036</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J93" s="20">
+        <f t="shared" si="1"/>
+        <v>0.49776738180353691</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="17">
         <v>45796</v>
       </c>
@@ -21626,8 +22021,12 @@
       <c r="I94" s="20">
         <v>-2.280214965622466</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J94" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.5585828715872877</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="17">
         <v>45797</v>
       </c>
@@ -21655,8 +22054,12 @@
       <c r="I95" s="20">
         <v>0.50444042759707231</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95" s="20">
+        <f t="shared" si="1"/>
+        <v>0.11806616573522349</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="17">
         <v>45798</v>
       </c>
@@ -21684,8 +22087,12 @@
       <c r="I96" s="20">
         <v>-2.7122704983830088</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J96" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.66356891798431772</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="17">
         <v>45799</v>
       </c>
@@ -21713,8 +22120,12 @@
       <c r="I97" s="20">
         <v>1.900421282743751</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J97" s="20">
+        <f t="shared" si="1"/>
+        <v>0.45727837276653932</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="17">
         <v>45800</v>
       </c>
@@ -21742,8 +22153,12 @@
       <c r="I98" s="20">
         <v>-0.49972178421616059</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J98" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.12593723791519709</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="17">
         <v>45804</v>
       </c>
@@ -21771,8 +22186,12 @@
       <c r="I99" s="20">
         <v>6.7097203424067162</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J99" s="20">
+        <f t="shared" si="1"/>
+        <v>1.6258996631570113</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="17">
         <v>45805</v>
       </c>
@@ -21800,8 +22219,12 @@
       <c r="I100" s="20">
         <v>-1.6644127542745959</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J100" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.40894784870287471</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="17">
         <v>45806</v>
       </c>
@@ -21829,8 +22252,12 @@
       <c r="I101" s="20">
         <v>0.4277752458705662</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J101" s="20">
+        <f t="shared" si="1"/>
+        <v>9.9437138410079715E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="17">
         <v>45807</v>
       </c>
@@ -21858,8 +22285,12 @@
       <c r="I102" s="20">
         <v>-3.3966011104025542</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J102" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.8298557953339718</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="17">
         <v>45810</v>
       </c>
@@ -21887,8 +22318,12 @@
       <c r="I103" s="20">
         <v>-1.094112343682941</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J103" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.27036940027040363</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="17">
         <v>45811</v>
       </c>
@@ -21916,8 +22351,12 @@
       <c r="I104" s="20">
         <v>0.45999848202144727</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J104" s="20">
+        <f t="shared" si="1"/>
+        <v>0.1072671276338812</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="17">
         <v>45812</v>
       </c>
@@ -21945,8 +22384,12 @@
       <c r="I105" s="20">
         <v>-3.6140673247457191</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J105" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.88269834990778706</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="17">
         <v>45813</v>
       </c>
@@ -21974,8 +22417,12 @@
       <c r="I106" s="20">
         <v>-15.38495657027309</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J106" s="20">
+        <f t="shared" si="1"/>
+        <v>-3.7429304977741591</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="17">
         <v>45814</v>
       </c>
@@ -22003,8 +22450,12 @@
       <c r="I107" s="20">
         <v>3.601382575131153</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J107" s="20">
+        <f t="shared" si="1"/>
+        <v>0.8705983921194872</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="17">
         <v>45817</v>
       </c>
@@ -22032,8 +22483,12 @@
       <c r="I108" s="20">
         <v>4.4531308979576476</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J108" s="20">
+        <f t="shared" si="1"/>
+        <v>1.0775664371009055</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="17">
         <v>45818</v>
       </c>
@@ -22061,8 +22516,12 @@
       <c r="I109" s="20">
         <v>5.519228787015023</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J109" s="20">
+        <f t="shared" si="1"/>
+        <v>1.3366197160375868</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="17">
         <v>45819</v>
       </c>
@@ -22090,8 +22549,12 @@
       <c r="I110" s="20">
         <v>0.1042113746000277</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J110" s="20">
+        <f t="shared" si="1"/>
+        <v>2.0813699926216313E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="17">
         <v>45820</v>
       </c>
@@ -22119,8 +22582,12 @@
       <c r="I111" s="20">
         <v>-2.2679659699347212</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J111" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.55560646338954023</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="17">
         <v>45821</v>
       </c>
@@ -22148,8 +22615,12 @@
       <c r="I112" s="20">
         <v>1.9242702929728019</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J112" s="20">
+        <f t="shared" si="1"/>
+        <v>0.46307349192271052</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="17">
         <v>45824</v>
       </c>
@@ -22177,8 +22648,12 @@
       <c r="I113" s="20">
         <v>1.167423563609808</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J113" s="20">
+        <f t="shared" si="1"/>
+        <v>0.27916577678095894</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="17">
         <v>45825</v>
       </c>
@@ -22206,8 +22681,12 @@
       <c r="I114" s="20">
         <v>-3.9603613904615851</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J114" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.9668450442412021</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="17">
         <v>45826</v>
       </c>
@@ -22235,8 +22714,12 @@
       <c r="I115" s="20">
         <v>1.7857617400006469</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J115" s="20">
+        <f t="shared" si="1"/>
+        <v>0.42941701893228268</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="17">
         <v>45828</v>
       </c>
@@ -22264,8 +22747,12 @@
       <c r="I116" s="20">
         <v>3.415035502990741E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J116" s="20">
+        <f t="shared" si="1"/>
+        <v>3.7894312998764364E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="17">
         <v>45831</v>
       </c>
@@ -22293,8 +22780,12 @@
       <c r="I117" s="20">
         <v>7.9106279600176421</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J117" s="20">
+        <f t="shared" si="1"/>
+        <v>1.9177106302692495</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="17">
         <v>45832</v>
       </c>
@@ -22322,8 +22813,12 @@
       <c r="I118" s="20">
         <v>-2.3827580162217972</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J118" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.58350001452752387</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="17">
         <v>45833</v>
       </c>
@@ -22351,8 +22846,12 @@
       <c r="I119" s="20">
         <v>-3.868630080327192</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J119" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.94455506794973487</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="17">
         <v>45834</v>
       </c>
@@ -22380,8 +22879,12 @@
       <c r="I120" s="20">
         <v>-0.5418408248426464</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J120" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.1361718286520813</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="17">
         <v>45835</v>
       </c>
@@ -22409,8 +22912,12 @@
       <c r="I121" s="20">
         <v>-0.66214189964193904</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J121" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.16540402975316282</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="17">
         <v>45838</v>
       </c>
@@ -22438,8 +22945,12 @@
       <c r="I122" s="20">
         <v>-1.8619259526030429</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J122" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.45694197962221794</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="17">
         <v>45839</v>
       </c>
@@ -22467,8 +22978,12 @@
       <c r="I123" s="20">
         <v>-5.4835283228870892</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J123" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.3369624530296529</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="17">
         <v>45840</v>
       </c>
@@ -22496,8 +23011,12 @@
       <c r="I124" s="20">
         <v>4.8487659635496412</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J124" s="20">
+        <f t="shared" si="1"/>
+        <v>1.173702600633276</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="17">
         <v>45841</v>
       </c>
@@ -22525,8 +23044,12 @@
       <c r="I125" s="20">
         <v>-9.5087170397421802E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J125" s="20">
+        <f t="shared" si="1"/>
+        <v>-2.761425598555119E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="17">
         <v>45845</v>
       </c>
@@ -22554,8 +23077,12 @@
       <c r="I126" s="20">
         <v>-7.0307468231121826</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J126" s="20">
+        <f t="shared" si="1"/>
+        <v>-1.7129242008473839</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="17">
         <v>45846</v>
       </c>
@@ -22583,8 +23110,12 @@
       <c r="I127" s="20">
         <v>1.3080034391201649</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J127" s="20">
+        <f t="shared" si="1"/>
+        <v>0.31332556461776656</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="17">
         <v>45847</v>
       </c>
@@ -22612,8 +23143,12 @@
       <c r="I128" s="20">
         <v>-0.65017325500732703</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J128" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.16249574462395616</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="17">
         <v>45848</v>
       </c>
@@ -22641,8 +23176,12 @@
       <c r="I129" s="20">
         <v>4.6198887966984872</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J129" s="20">
+        <f t="shared" si="1"/>
+        <v>1.1180872756663036</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="17">
         <v>45849</v>
       </c>
@@ -22670,8 +23209,12 @@
       <c r="I130" s="20">
         <v>1.1678402804230399</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J130" s="20">
+        <f t="shared" si="1"/>
+        <v>0.27926703564092276</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="17">
         <v>45852</v>
       </c>
@@ -22699,8 +23242,12 @@
       <c r="I131" s="20">
         <v>1.075500920599292</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J131" s="20">
+        <f t="shared" ref="J131:J194" si="2">(H131-C$227)/C$228</f>
+        <v>0.25682930812754562</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="17">
         <v>45853</v>
       </c>
@@ -22728,8 +23275,12 @@
       <c r="I132" s="20">
         <v>-1.950100033828696</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J132" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.47836757767769383</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="17">
         <v>45854</v>
       </c>
@@ -22757,8 +23308,12 @@
       <c r="I133" s="20">
         <v>3.444090895289647</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J133" s="20">
+        <f t="shared" si="2"/>
+        <v>0.83237776920049</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="17">
         <v>45855</v>
       </c>
@@ -22786,8 +23341,12 @@
       <c r="I134" s="20">
         <v>-0.70506313168599444</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J134" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.17583354660254502</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="17">
         <v>45856</v>
       </c>
@@ -22815,8 +23374,12 @@
       <c r="I135" s="20">
         <v>3.1555941564684051</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J135" s="20">
+        <f t="shared" si="2"/>
+        <v>0.7622753640449349</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="17">
         <v>45859</v>
       </c>
@@ -22844,8 +23407,12 @@
       <c r="I136" s="20">
         <v>-0.35250894982966557</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J136" s="20">
+        <f t="shared" si="2"/>
+        <v>-9.0165694006500999E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="17">
         <v>45860</v>
       </c>
@@ -22873,8 +23440,12 @@
       <c r="I137" s="20">
         <v>1.095984328057463</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J137" s="20">
+        <f t="shared" si="2"/>
+        <v>0.26180661266993333</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="17">
         <v>45861</v>
       </c>
@@ -22902,8 +23473,12 @@
       <c r="I138" s="20">
         <v>0.13540556027952949</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J138" s="20">
+        <f t="shared" si="2"/>
+        <v>2.8393638097916132E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="17">
         <v>45862</v>
       </c>
@@ -22931,8 +23506,12 @@
       <c r="I139" s="20">
         <v>-8.5525395203549799</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J139" s="20">
+        <f t="shared" si="2"/>
+        <v>-2.0827076814536625</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="17">
         <v>45863</v>
       </c>
@@ -22960,8 +23539,12 @@
       <c r="I140" s="20">
         <v>3.4637169240125409</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J140" s="20">
+        <f t="shared" si="2"/>
+        <v>0.83714673755260482</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="17">
         <v>45866</v>
       </c>
@@ -22989,8 +23572,12 @@
       <c r="I141" s="20">
         <v>2.9706852145075562</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J141" s="20">
+        <f t="shared" si="2"/>
+        <v>0.71734396683334889</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="17">
         <v>45867</v>
       </c>
@@ -23018,8 +23605,12 @@
       <c r="I142" s="20">
         <v>-1.3574939053426569</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J142" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.33436901780997186</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="17">
         <v>45868</v>
       </c>
@@ -23047,8 +23638,12 @@
       <c r="I143" s="20">
         <v>-0.67474952991329695</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J143" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.16846758329260789</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="17">
         <v>45869</v>
       </c>
@@ -23076,8 +23671,12 @@
       <c r="I144" s="20">
         <v>-3.4340464433143079</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J144" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.83895471239518293</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="17">
         <v>45870</v>
       </c>
@@ -23105,8 +23704,12 @@
       <c r="I145" s="20">
         <v>-1.846508512028987</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J145" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.45319566460319849</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="17">
         <v>45873</v>
       </c>
@@ -23134,8 +23737,12 @@
       <c r="I146" s="20">
         <v>2.1671409827243679</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J146" s="20">
+        <f t="shared" si="2"/>
+        <v>0.52208913127772894</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="17">
         <v>45874</v>
       </c>
@@ -23163,8 +23770,12 @@
       <c r="I147" s="20">
         <v>-0.17476298179210409</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J147" s="20">
+        <f t="shared" si="2"/>
+        <v>-4.6974842293420929E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="17">
         <v>45875</v>
       </c>
@@ -23192,8 +23803,12 @@
       <c r="I148" s="20">
         <v>3.5604989006210408</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J148" s="20">
+        <f t="shared" si="2"/>
+        <v>0.86066398548991496</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="17">
         <v>45876</v>
       </c>
@@ -23221,8 +23836,12 @@
       <c r="I149" s="20">
         <v>0.73499972730621921</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J149" s="20">
+        <f t="shared" si="2"/>
+        <v>0.17409023556225331</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="17">
         <v>45877</v>
       </c>
@@ -23250,8 +23869,12 @@
       <c r="I150" s="20">
         <v>2.264178205067275</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J150" s="20">
+        <f t="shared" si="2"/>
+        <v>0.54566840189148491</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="17">
         <v>45880</v>
       </c>
@@ -23279,8 +23902,12 @@
       <c r="I151" s="20">
         <v>2.8057113480860441</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J151" s="20">
+        <f t="shared" si="2"/>
+        <v>0.67725663388389334</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="17">
         <v>45881</v>
       </c>
@@ -23308,8 +23935,12 @@
       <c r="I152" s="20">
         <v>0.53245599195861881</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J152" s="20">
+        <f t="shared" si="2"/>
+        <v>0.12487372429397574</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="17">
         <v>45882</v>
       </c>
@@ -23337,8 +23968,12 @@
       <c r="I153" s="20">
         <v>-0.42927354150751101</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J153" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.1088188771564688</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="17">
         <v>45883</v>
       </c>
@@ -23366,8 +24001,12 @@
       <c r="I154" s="20">
         <v>-1.1260045483128449</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J154" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.27811895147643889</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="17">
         <v>45884</v>
       </c>
@@ -23395,8 +24034,12 @@
       <c r="I155" s="20">
         <v>-1.5072192130277871</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J155" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.37075107267918378</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="17">
         <v>45887</v>
       </c>
@@ -23424,8 +24067,12 @@
       <c r="I156" s="20">
         <v>1.3819843813812049</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J156" s="20">
+        <f t="shared" si="2"/>
+        <v>0.33130234317465224</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="17">
         <v>45888</v>
       </c>
@@ -23453,8 +24100,12 @@
       <c r="I157" s="20">
         <v>-1.7608473377750991</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J157" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.43238068288734793</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="17">
         <v>45889</v>
       </c>
@@ -23482,8 +24133,12 @@
       <c r="I158" s="20">
         <v>-1.656473019005132</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J158" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.40701855639627166</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="17">
         <v>45890</v>
       </c>
@@ -23511,8 +24166,12 @@
       <c r="I159" s="20">
         <v>-1.1770139452006401</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J159" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.29051382783441532</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="17">
         <v>45891</v>
       </c>
@@ -23540,8 +24199,12 @@
       <c r="I160" s="20">
         <v>6.0310342217118329</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J160" s="20">
+        <f t="shared" si="2"/>
+        <v>1.4609843521528043</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="17">
         <v>45894</v>
       </c>
@@ -23569,8 +24232,12 @@
       <c r="I161" s="20">
         <v>1.919634833911025</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J161" s="20">
+        <f t="shared" si="2"/>
+        <v>0.46194711236445829</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="17">
         <v>45895</v>
       </c>
@@ -23598,8 +24265,12 @@
       <c r="I162" s="20">
         <v>1.4521858588614891</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J162" s="20">
+        <f t="shared" si="2"/>
+        <v>0.348360741952223</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="17">
         <v>45896</v>
       </c>
@@ -23627,8 +24298,12 @@
       <c r="I163" s="20">
         <v>-0.59035920887402127</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J163" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.14796140876573288</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="17">
         <v>45897</v>
       </c>
@@ -23656,8 +24331,12 @@
       <c r="I164" s="20">
         <v>-1.04086738625491</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J164" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.25743130054227181</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="17">
         <v>45898</v>
       </c>
@@ -23685,8 +24364,12 @@
       <c r="I165" s="20">
         <v>-3.562927426538796</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J165" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.87027176277074203</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="17">
         <v>45902</v>
       </c>
@@ -23714,8 +24397,12 @@
       <c r="I166" s="20">
         <v>-1.360031819179417</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J166" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.33498571061822097</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="17">
         <v>45903</v>
       </c>
@@ -23743,8 +24430,12 @@
       <c r="I167" s="20">
         <v>1.4259040294779579</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J167" s="20">
+        <f t="shared" si="2"/>
+        <v>0.34197446715687752</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="17">
         <v>45904</v>
       </c>
@@ -23772,8 +24463,12 @@
       <c r="I168" s="20">
         <v>1.320229696128955</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J168" s="20">
+        <f t="shared" si="2"/>
+        <v>0.31629644749799629</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="17">
         <v>45905</v>
       </c>
@@ -23801,8 +24496,12 @@
       <c r="I169" s="20">
         <v>3.5717564365462211</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J169" s="20">
+        <f t="shared" si="2"/>
+        <v>0.86339947687780605</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="17">
         <v>45908</v>
       </c>
@@ -23830,8 +24529,12 @@
       <c r="I170" s="20">
         <v>-1.273610239490075</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J170" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.31398595645004945</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="17">
         <v>45909</v>
       </c>
@@ -23859,8 +24562,12 @@
       <c r="I171" s="20">
         <v>0.16441441896894679</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J171" s="20">
+        <f t="shared" si="2"/>
+        <v>3.5442559251253065E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="17">
         <v>45910</v>
       </c>
@@ -23888,8 +24595,12 @@
       <c r="I172" s="20">
         <v>0.23605284724501349</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J172" s="20">
+        <f t="shared" si="2"/>
+        <v>5.2850125604464906E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="17">
         <v>45911</v>
       </c>
@@ -23917,8 +24628,12 @@
       <c r="I173" s="20">
         <v>5.8682756931876883</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J173" s="20">
+        <f t="shared" si="2"/>
+        <v>1.421435328632676</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="17">
         <v>45912</v>
       </c>
@@ -23946,8 +24661,12 @@
       <c r="I174" s="20">
         <v>7.0981078341088466</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J174" s="20">
+        <f t="shared" si="2"/>
+        <v>1.7202747240741565</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="17">
         <v>45915</v>
       </c>
@@ -23975,8 +24694,12 @@
       <c r="I175" s="20">
         <v>3.499203129181562</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J175" s="20">
+        <f t="shared" si="2"/>
+        <v>0.84576960220735309</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="17">
         <v>45916</v>
       </c>
@@ -24004,8 +24727,12 @@
       <c r="I176" s="20">
         <v>2.784971851696056</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J176" s="20">
+        <f t="shared" si="2"/>
+        <v>0.67221710177481797</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="17">
         <v>45917</v>
       </c>
@@ -24033,8 +24760,12 @@
       <c r="I177" s="20">
         <v>1.0006219326091239</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J177" s="20">
+        <f t="shared" si="2"/>
+        <v>0.23863431162542847</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="17">
         <v>45918</v>
       </c>
@@ -24062,8 +24793,12 @@
       <c r="I178" s="20">
         <v>-2.1384208901630082</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J178" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.5241280428528966</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="17">
         <v>45919</v>
       </c>
@@ -24091,8 +24826,12 @@
       <c r="I179" s="20">
         <v>2.187720716264518</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J179" s="20">
+        <f t="shared" si="2"/>
+        <v>0.52708984228929745</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="17">
         <v>45922</v>
       </c>
@@ -24120,8 +24859,12 @@
       <c r="I180" s="20">
         <v>1.892463602107167</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J180" s="20">
+        <f t="shared" si="2"/>
+        <v>0.45534471987894121</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="17">
         <v>45923</v>
       </c>
@@ -24149,8 +24892,12 @@
       <c r="I181" s="20">
         <v>-1.944111645324947</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J181" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.47691244706223551</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="17">
         <v>45924</v>
       </c>
@@ -24178,8 +24925,12 @@
       <c r="I182" s="20">
         <v>3.9008445433210519</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J182" s="20">
+        <f t="shared" si="2"/>
+        <v>0.94336526050248071</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="17">
         <v>45925</v>
       </c>
@@ -24207,8 +24958,12 @@
       <c r="I183" s="20">
         <v>-4.4801876926275224</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J183" s="20">
+        <f t="shared" si="2"/>
+        <v>-1.0931586871400567</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="17">
         <v>45926</v>
       </c>
@@ -24236,8 +24991,12 @@
       <c r="I184" s="20">
         <v>3.938966475449968</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J184" s="20">
+        <f t="shared" si="2"/>
+        <v>0.95262858577379261</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="17">
         <v>45929</v>
       </c>
@@ -24265,8 +25024,12 @@
       <c r="I185" s="20">
         <v>0.63602935068997302</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J185" s="20">
+        <f t="shared" si="2"/>
+        <v>0.15004122388781316</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="17">
         <v>45930</v>
       </c>
@@ -24294,8 +25057,12 @@
       <c r="I186" s="20">
         <v>0.34011722897895208</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J186" s="20">
+        <f t="shared" si="2"/>
+        <v>7.8136939869270575E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="17">
         <v>45931</v>
       </c>
@@ -24323,8 +25090,12 @@
       <c r="I187" s="20">
         <v>3.2607016218810672</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J187" s="20">
+        <f t="shared" si="2"/>
+        <v>0.78781563931923337</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="17">
         <v>45932</v>
       </c>
@@ -24352,8 +25123,12 @@
       <c r="I188" s="20">
         <v>-5.2409643514990556</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J188" s="20">
+        <f t="shared" si="2"/>
+        <v>-1.2780213437891752</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="17">
         <v>45933</v>
       </c>
@@ -24381,8 +25156,12 @@
       <c r="I189" s="20">
         <v>-1.4252461669591019</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J189" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.35083227667884986</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="17">
         <v>45936</v>
       </c>
@@ -24410,8 +25189,12 @@
       <c r="I190" s="20">
         <v>5.3054067955517086</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J190" s="20">
+        <f t="shared" si="2"/>
+        <v>1.284662678540478</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="17">
         <v>45937</v>
       </c>
@@ -24439,8 +25222,12 @@
       <c r="I191" s="20">
         <v>-4.5498291036749761</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J191" s="20">
+        <f t="shared" si="2"/>
+        <v>-1.1100809942441177</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="17">
         <v>45938</v>
       </c>
@@ -24468,8 +25255,12 @@
       <c r="I192" s="20">
         <v>1.284745469368666</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J192" s="20">
+        <f t="shared" si="2"/>
+        <v>0.30767406358078064</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="17">
         <v>45939</v>
       </c>
@@ -24497,8 +25288,12 @@
       <c r="I193" s="20">
         <v>-0.72063727670931166</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J193" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.17961793955213898</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="17">
         <v>45940</v>
       </c>
@@ -24526,8 +25321,12 @@
       <c r="I194" s="20">
         <v>-5.1953310150347107</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J194" s="20">
+        <f t="shared" si="2"/>
+        <v>-1.266932807209892</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="17">
         <v>45943</v>
       </c>
@@ -24555,8 +25354,12 @@
       <c r="I195" s="20">
         <v>5.2779528869889569</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J195" s="20">
+        <f t="shared" ref="J195:J223" si="3">(H195-C$227)/C$228</f>
+        <v>1.2779915978584806</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="17">
         <v>45944</v>
       </c>
@@ -24584,8 +25387,12 @@
       <c r="I196" s="20">
         <v>-1.5396656185420139</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J196" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.37863529027725212</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="17">
         <v>45945</v>
       </c>
@@ -24613,8 +25420,12 @@
       <c r="I197" s="20">
         <v>1.3674596176595899</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J197" s="20">
+        <f t="shared" si="3"/>
+        <v>0.32777294150667607</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="17">
         <v>45946</v>
       </c>
@@ -24642,8 +25453,12 @@
       <c r="I198" s="20">
         <v>-1.481680075537301</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J198" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.36454526608671894</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="17">
         <v>45947</v>
       </c>
@@ -24671,8 +25486,12 @@
       <c r="I199" s="20">
         <v>2.433131572986619</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J199" s="20">
+        <f t="shared" si="3"/>
+        <v>0.58672272194609121</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="17">
         <v>45950</v>
       </c>
@@ -24700,8 +25519,12 @@
       <c r="I200" s="20">
         <v>1.831478668828783</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J200" s="20">
+        <f t="shared" si="3"/>
+        <v>0.44052586778884961</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="17">
         <v>45951</v>
       </c>
@@ -24729,8 +25552,12 @@
       <c r="I201" s="20">
         <v>-1.0853673281354379</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J201" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.2682444312828598</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="17">
         <v>45952</v>
       </c>
@@ -24758,8 +25585,12 @@
       <c r="I202" s="20">
         <v>-0.82353540067065023</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J202" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.20462136248564342</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="17">
         <v>45953</v>
       </c>
@@ -24787,8 +25618,12 @@
       <c r="I203" s="20">
         <v>2.2547269710079458</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J203" s="20">
+        <f t="shared" si="3"/>
+        <v>0.54337182744161705</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="17">
         <v>45954</v>
       </c>
@@ -24816,8 +25651,12 @@
       <c r="I204" s="20">
         <v>-3.4579178716340908</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J204" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.84475527896849234</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" s="17">
         <v>45957</v>
       </c>
@@ -24845,8 +25684,12 @@
       <c r="I205" s="20">
         <v>4.2211787325708316</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J205" s="20">
+        <f t="shared" si="3"/>
+        <v>1.0212039120301106</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" s="17">
         <v>45958</v>
       </c>
@@ -24874,8 +25717,12 @@
       <c r="I206" s="20">
         <v>1.7810475504555161</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J206" s="20">
+        <f t="shared" si="3"/>
+        <v>0.42827150849489215</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" s="17">
         <v>45959</v>
       </c>
@@ -24903,8 +25750,12 @@
       <c r="I207" s="20">
         <v>0.2082294746276922</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J207" s="20">
+        <f t="shared" si="3"/>
+        <v>4.6089268105753312E-2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" s="17">
         <v>45960</v>
       </c>
@@ -24932,8 +25783,12 @@
       <c r="I208" s="20">
         <v>-4.7501748363475809</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J208" s="20">
+        <f t="shared" si="3"/>
+        <v>-1.1587634084037586</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" s="17">
         <v>45961</v>
       </c>
@@ -24961,8 +25816,12 @@
       <c r="I209" s="20">
         <v>3.6718152411406848</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J209" s="20">
+        <f t="shared" si="3"/>
+        <v>0.88771296786464127</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" s="17">
         <v>45964</v>
       </c>
@@ -24990,8 +25849,12 @@
       <c r="I210" s="20">
         <v>2.553845562158628</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J210" s="20">
+        <f t="shared" si="3"/>
+        <v>0.61605525794443694</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" s="17">
         <v>45965</v>
       </c>
@@ -25019,8 +25882,12 @@
       <c r="I211" s="20">
         <v>-5.2848605220562446</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J211" s="20">
+        <f t="shared" si="3"/>
+        <v>-1.2886877629166515</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" s="17">
         <v>45966</v>
       </c>
@@ -25048,8 +25915,12 @@
       <c r="I212" s="20">
         <v>3.930641812651638</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J212" s="20">
+        <f t="shared" si="3"/>
+        <v>0.9506057591496293</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" s="17">
         <v>45967</v>
       </c>
@@ -25077,8 +25948,12 @@
       <c r="I213" s="20">
         <v>-3.5599256820994301</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J213" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.86954236282770758</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" s="17">
         <v>45968</v>
       </c>
@@ -25106,8 +25981,12 @@
       <c r="I214" s="20">
         <v>-3.7448831820684378</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J214" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.9144855592477541</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" s="17">
         <v>45971</v>
       </c>
@@ -25135,8 +26014,12 @@
       <c r="I215" s="20">
         <v>3.5922696461522552</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J215" s="20">
+        <f t="shared" si="3"/>
+        <v>0.86838402310428542</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" s="17">
         <v>45972</v>
       </c>
@@ -25164,8 +26047,12 @@
       <c r="I216" s="20">
         <v>-1.2680285175909181</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J216" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.31262964257406217</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" s="17">
         <v>45973</v>
       </c>
@@ -25193,8 +26080,12 @@
       <c r="I217" s="20">
         <v>-2.073113246966483</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J217" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.50825880675052948</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" s="17">
         <v>45974</v>
       </c>
@@ -25222,8 +26113,12 @@
       <c r="I218" s="20">
         <v>-6.8752372242535609</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J218" s="20">
+        <f t="shared" si="3"/>
+        <v>-1.6751366093851465</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" s="17">
         <v>45975</v>
       </c>
@@ -25251,8 +26146,12 @@
       <c r="I219" s="20">
         <v>0.58536268541041414</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J219" s="20">
+        <f t="shared" si="3"/>
+        <v>0.13772962857543314</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" s="17">
         <v>45978</v>
       </c>
@@ -25280,8 +26179,12 @@
       <c r="I220" s="20">
         <v>1.1238698346982099</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J220" s="20">
+        <f t="shared" si="3"/>
+        <v>0.26858256824047039</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" s="17">
         <v>45979</v>
       </c>
@@ -25309,8 +26212,12 @@
       <c r="I221" s="20">
         <v>-1.893486344458768</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J221" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.46461090297219382</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" s="17">
         <v>45980</v>
       </c>
@@ -25338,8 +26245,12 @@
       <c r="I222" s="20">
         <v>0.68054507353294491</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J222" s="20">
+        <f t="shared" si="3"/>
+        <v>0.16085818927633364</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" s="17">
         <v>45981</v>
       </c>
@@ -25366,6 +26277,10 @@
       </c>
       <c r="I223" s="20">
         <v>-2.192225125575701</v>
+      </c>
+      <c r="J223" s="20">
+        <f t="shared" si="3"/>
+        <v>-0.53720204266792582</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.35">
@@ -25404,7 +26319,7 @@
         <v>4.1153614941039043E-2</v>
       </c>
       <c r="D228" s="21">
-        <f t="shared" ref="D228:D233" si="0">C228</f>
+        <f t="shared" ref="D228:D233" si="4">C228</f>
         <v>4.1153614941039043E-2</v>
       </c>
     </row>
@@ -25416,7 +26331,7 @@
         <v>-0.16754566208266</v>
       </c>
       <c r="D229" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.16754566208266</v>
       </c>
     </row>
@@ -25428,7 +26343,7 @@
         <v>-2.188083285261834E-2</v>
       </c>
       <c r="D230" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-2.188083285261834E-2</v>
       </c>
     </row>
@@ -25440,7 +26355,7 @@
         <v>2.5001306014088407E-4</v>
       </c>
       <c r="D231" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.5001306014088407E-4</v>
       </c>
     </row>
@@ -25452,7 +26367,7 @@
         <v>2.4271243897543739E-2</v>
       </c>
       <c r="D232" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.4271243897543739E-2</v>
       </c>
     </row>
@@ -25464,7 +26379,7 @@
         <v>0.20449053790685209</v>
       </c>
       <c r="D233" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.20449053790685209</v>
       </c>
     </row>
@@ -25494,7 +26409,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I223">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -25506,7 +26421,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B223">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>